<commit_message>
inicio funcao OU e uso de DATA em valores lógicos
</commit_message>
<xml_diff>
--- a/2.Excel/hands-on/6.Funcoes_Mercado/2.E_OU/1.Funcao_E.xlsx
+++ b/2.Excel/hands-on/6.Funcoes_Mercado/2.E_OU/1.Funcao_E.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Projetos para Github\Hashtag\2.Excel\hands-on\6.Funcoes_Mercado\2.E_OU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C393C9C8-3CA0-45DC-B00B-65420169294F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408CC8D1-CA4F-45A0-A81B-41C6349EAB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="957" xr2:uid="{85B08948-7BCF-4007-BABB-111144F4B1B5}"/>
+    <workbookView xWindow="12144" yWindow="156" windowWidth="10896" windowHeight="12792" tabRatio="506" xr2:uid="{85B08948-7BCF-4007-BABB-111144F4B1B5}"/>
   </bookViews>
   <sheets>
     <sheet name="PraticaE" sheetId="8" r:id="rId1"/>
@@ -3441,7 +3441,7 @@
   <dimension ref="A1:M1999"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3497,7 +3497,7 @@
         <v>Não</v>
       </c>
       <c r="G2" s="12" t="str">
-        <f>IF(AND(B2&lt;"31/12/2010",C2="Concurso",D2="RJ"),"Sim","Não")</f>
+        <f>IF(AND(B2&lt;DATE(2010,12,31),C2="Concurso",D2="RJ"),"Sim","Não")</f>
         <v>Sim</v>
       </c>
     </row>
@@ -3522,7 +3522,7 @@
         <v>Sim</v>
       </c>
       <c r="G3" s="12" t="str">
-        <f t="shared" ref="G3:G66" si="1">IF(AND(B3&lt;"31/12/2010",C3="Concurso",D3="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G3:G66" si="1">IF(AND(B3&lt;DATE(2010,12,31),C3="Concurso",D3="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
       <c r="I3" s="24" t="s">
@@ -3931,8 +3931,8 @@
         <v>Não</v>
       </c>
       <c r="G17" s="12" t="str">
-        <f>IF(AND(B17&lt;"31/12/2010",C17="Concurso",D17="RJ"),"Sim","Não")</f>
-        <v>Sim</v>
+        <f t="shared" si="1"/>
+        <v>Não</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -4257,7 +4257,7 @@
       </c>
       <c r="G30" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4857,7 +4857,7 @@
       </c>
       <c r="G54" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -5181,7 +5181,7 @@
         <v>Não</v>
       </c>
       <c r="G67" s="12" t="str">
-        <f t="shared" ref="G67:G130" si="3">IF(AND(B67&lt;"31/12/2010",C67="Concurso",D67="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G67:G130" si="3">IF(AND(B67&lt;DATE(2010,12,31),C67="Concurso",D67="RJ"),"Sim","Não")</f>
         <v>Sim</v>
       </c>
     </row>
@@ -5732,7 +5732,7 @@
       </c>
       <c r="G89" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -5882,7 +5882,7 @@
       </c>
       <c r="G95" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -5932,7 +5932,7 @@
       </c>
       <c r="G97" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.3">
@@ -6057,7 +6057,7 @@
       </c>
       <c r="G102" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.3">
@@ -6132,7 +6132,7 @@
       </c>
       <c r="G105" s="12" t="str">
         <f t="shared" si="3"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.3">
@@ -6781,7 +6781,7 @@
         <v>Não</v>
       </c>
       <c r="G131" s="12" t="str">
-        <f t="shared" ref="G131:G194" si="5">IF(AND(B131&lt;"31/12/2010",C131="Concurso",D131="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G131:G194" si="5">IF(AND(B131&lt;DATE(2010,12,31),C131="Concurso",D131="RJ"),"Sim","Não")</f>
         <v>Sim</v>
       </c>
     </row>
@@ -7607,7 +7607,7 @@
       </c>
       <c r="G164" s="12" t="str">
         <f t="shared" si="5"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.3">
@@ -8381,7 +8381,7 @@
         <v>Sim</v>
       </c>
       <c r="G195" s="12" t="str">
-        <f t="shared" ref="G195:G258" si="7">IF(AND(B195&lt;"31/12/2010",C195="Concurso",D195="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G195:G258" si="7">IF(AND(B195&lt;DATE(2010,12,31),C195="Concurso",D195="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -8457,7 +8457,7 @@
       </c>
       <c r="G198" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.3">
@@ -8482,7 +8482,7 @@
       </c>
       <c r="G199" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.3">
@@ -9557,7 +9557,7 @@
       </c>
       <c r="G242" s="12" t="str">
         <f t="shared" si="7"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.3">
@@ -9981,7 +9981,7 @@
         <v>Não</v>
       </c>
       <c r="G259" s="12" t="str">
-        <f t="shared" ref="G259:G322" si="9">IF(AND(B259&lt;"31/12/2010",C259="Concurso",D259="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G259:G322" si="9">IF(AND(B259&lt;DATE(2010,12,31),C259="Concurso",D259="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -10232,7 +10232,7 @@
       </c>
       <c r="G269" s="12" t="str">
         <f t="shared" si="9"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.3">
@@ -10507,7 +10507,7 @@
       </c>
       <c r="G280" s="12" t="str">
         <f t="shared" si="9"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.3">
@@ -11082,7 +11082,7 @@
       </c>
       <c r="G303" s="12" t="str">
         <f t="shared" si="9"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="304" spans="1:7" x14ac:dyDescent="0.3">
@@ -11581,7 +11581,7 @@
         <v>Não</v>
       </c>
       <c r="G323" s="12" t="str">
-        <f t="shared" ref="G323:G386" si="11">IF(AND(B323&lt;"31/12/2010",C323="Concurso",D323="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G323:G386" si="11">IF(AND(B323&lt;DATE(2010,12,31),C323="Concurso",D323="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -11857,7 +11857,7 @@
       </c>
       <c r="G334" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.3">
@@ -12082,7 +12082,7 @@
       </c>
       <c r="G343" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="344" spans="1:7" x14ac:dyDescent="0.3">
@@ -12832,7 +12832,7 @@
       </c>
       <c r="G373" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="374" spans="1:7" x14ac:dyDescent="0.3">
@@ -12882,7 +12882,7 @@
       </c>
       <c r="G375" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="376" spans="1:7" x14ac:dyDescent="0.3">
@@ -13181,7 +13181,7 @@
         <v>Não</v>
       </c>
       <c r="G387" s="12" t="str">
-        <f t="shared" ref="G387:G450" si="13">IF(AND(B387&lt;"31/12/2010",C387="Concurso",D387="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G387:G450" si="13">IF(AND(B387&lt;DATE(2010,12,31),C387="Concurso",D387="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -13207,7 +13207,7 @@
       </c>
       <c r="G388" s="12" t="str">
         <f t="shared" si="13"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="389" spans="1:7" x14ac:dyDescent="0.3">
@@ -13332,7 +13332,7 @@
       </c>
       <c r="G393" s="12" t="str">
         <f t="shared" si="13"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="394" spans="1:7" x14ac:dyDescent="0.3">
@@ -13357,7 +13357,7 @@
       </c>
       <c r="G394" s="12" t="str">
         <f t="shared" si="13"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="395" spans="1:7" x14ac:dyDescent="0.3">
@@ -13782,7 +13782,7 @@
       </c>
       <c r="G411" s="12" t="str">
         <f t="shared" si="13"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="412" spans="1:7" x14ac:dyDescent="0.3">
@@ -14257,7 +14257,7 @@
       </c>
       <c r="G430" s="12" t="str">
         <f t="shared" si="13"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="431" spans="1:7" x14ac:dyDescent="0.3">
@@ -14781,7 +14781,7 @@
         <v>Não</v>
       </c>
       <c r="G451" s="12" t="str">
-        <f t="shared" ref="G451:G514" si="15">IF(AND(B451&lt;"31/12/2010",C451="Concurso",D451="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G451:G514" si="15">IF(AND(B451&lt;DATE(2010,12,31),C451="Concurso",D451="RJ"),"Sim","Não")</f>
         <v>Sim</v>
       </c>
     </row>
@@ -16007,7 +16007,7 @@
       </c>
       <c r="G500" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="501" spans="1:7" x14ac:dyDescent="0.3">
@@ -16207,7 +16207,7 @@
       </c>
       <c r="G508" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="509" spans="1:7" x14ac:dyDescent="0.3">
@@ -16332,7 +16332,7 @@
       </c>
       <c r="G513" s="12" t="str">
         <f t="shared" si="15"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="514" spans="1:7" x14ac:dyDescent="0.3">
@@ -16381,7 +16381,7 @@
         <v>Não</v>
       </c>
       <c r="G515" s="12" t="str">
-        <f t="shared" ref="G515:G578" si="17">IF(AND(B515&lt;"31/12/2010",C515="Concurso",D515="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G515:G578" si="17">IF(AND(B515&lt;DATE(2010,12,31),C515="Concurso",D515="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -16932,7 +16932,7 @@
       </c>
       <c r="G537" s="12" t="str">
         <f t="shared" si="17"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="538" spans="1:7" x14ac:dyDescent="0.3">
@@ -17482,7 +17482,7 @@
       </c>
       <c r="G559" s="12" t="str">
         <f t="shared" si="17"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="560" spans="1:7" x14ac:dyDescent="0.3">
@@ -17507,7 +17507,7 @@
       </c>
       <c r="G560" s="12" t="str">
         <f t="shared" si="17"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="561" spans="1:7" x14ac:dyDescent="0.3">
@@ -17807,7 +17807,7 @@
       </c>
       <c r="G572" s="12" t="str">
         <f t="shared" si="17"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="573" spans="1:7" x14ac:dyDescent="0.3">
@@ -17981,7 +17981,7 @@
         <v>Não</v>
       </c>
       <c r="G579" s="12" t="str">
-        <f t="shared" ref="G579:G642" si="19">IF(AND(B579&lt;"31/12/2010",C579="Concurso",D579="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G579:G642" si="19">IF(AND(B579&lt;DATE(2010,12,31),C579="Concurso",D579="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -18382,7 +18382,7 @@
       </c>
       <c r="G595" s="12" t="str">
         <f t="shared" si="19"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="596" spans="1:7" x14ac:dyDescent="0.3">
@@ -18882,7 +18882,7 @@
       </c>
       <c r="G615" s="12" t="str">
         <f t="shared" si="19"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="616" spans="1:7" x14ac:dyDescent="0.3">
@@ -19557,7 +19557,7 @@
       </c>
       <c r="G642" s="12" t="str">
         <f t="shared" si="19"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="643" spans="1:7" x14ac:dyDescent="0.3">
@@ -19581,7 +19581,7 @@
         <v>Não</v>
       </c>
       <c r="G643" s="12" t="str">
-        <f t="shared" ref="G643:G706" si="21">IF(AND(B643&lt;"31/12/2010",C643="Concurso",D643="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G643:G706" si="21">IF(AND(B643&lt;DATE(2010,12,31),C643="Concurso",D643="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -19832,7 +19832,7 @@
       </c>
       <c r="G653" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="654" spans="1:7" x14ac:dyDescent="0.3">
@@ -20132,7 +20132,7 @@
       </c>
       <c r="G665" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="666" spans="1:7" x14ac:dyDescent="0.3">
@@ -20157,7 +20157,7 @@
       </c>
       <c r="G666" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="667" spans="1:7" x14ac:dyDescent="0.3">
@@ -20632,7 +20632,7 @@
       </c>
       <c r="G685" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="686" spans="1:7" x14ac:dyDescent="0.3">
@@ -20932,7 +20932,7 @@
       </c>
       <c r="G697" s="12" t="str">
         <f t="shared" si="21"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="698" spans="1:7" x14ac:dyDescent="0.3">
@@ -21181,7 +21181,7 @@
         <v>Não</v>
       </c>
       <c r="G707" s="12" t="str">
-        <f t="shared" ref="G707:G770" si="23">IF(AND(B707&lt;"31/12/2010",C707="Concurso",D707="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G707:G770" si="23">IF(AND(B707&lt;DATE(2010,12,31),C707="Concurso",D707="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -21232,7 +21232,7 @@
       </c>
       <c r="G709" s="12" t="str">
         <f t="shared" si="23"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="710" spans="1:7" x14ac:dyDescent="0.3">
@@ -21482,7 +21482,7 @@
       </c>
       <c r="G719" s="12" t="str">
         <f t="shared" si="23"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="720" spans="1:7" x14ac:dyDescent="0.3">
@@ -21607,7 +21607,7 @@
       </c>
       <c r="G724" s="12" t="str">
         <f t="shared" si="23"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="725" spans="1:7" x14ac:dyDescent="0.3">
@@ -21857,7 +21857,7 @@
       </c>
       <c r="G734" s="12" t="str">
         <f t="shared" si="23"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="735" spans="1:7" x14ac:dyDescent="0.3">
@@ -22207,7 +22207,7 @@
       </c>
       <c r="G748" s="12" t="str">
         <f t="shared" si="23"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="749" spans="1:7" x14ac:dyDescent="0.3">
@@ -22582,7 +22582,7 @@
       </c>
       <c r="G763" s="12" t="str">
         <f t="shared" si="23"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="764" spans="1:7" x14ac:dyDescent="0.3">
@@ -22781,7 +22781,7 @@
         <v>Não</v>
       </c>
       <c r="G771" s="12" t="str">
-        <f t="shared" ref="G771:G834" si="25">IF(AND(B771&lt;"31/12/2010",C771="Concurso",D771="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G771:G834" si="25">IF(AND(B771&lt;DATE(2010,12,31),C771="Concurso",D771="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -24182,7 +24182,7 @@
       </c>
       <c r="G827" s="12" t="str">
         <f t="shared" si="25"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="828" spans="1:7" x14ac:dyDescent="0.3">
@@ -24381,7 +24381,7 @@
         <v>Não</v>
       </c>
       <c r="G835" s="12" t="str">
-        <f t="shared" ref="G835:G898" si="27">IF(AND(B835&lt;"31/12/2010",C835="Concurso",D835="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G835:G898" si="27">IF(AND(B835&lt;DATE(2010,12,31),C835="Concurso",D835="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -24407,7 +24407,7 @@
       </c>
       <c r="G836" s="12" t="str">
         <f t="shared" si="27"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="837" spans="1:7" x14ac:dyDescent="0.3">
@@ -25682,7 +25682,7 @@
       </c>
       <c r="G887" s="12" t="str">
         <f t="shared" si="27"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="888" spans="1:7" x14ac:dyDescent="0.3">
@@ -25757,7 +25757,7 @@
       </c>
       <c r="G890" s="12" t="str">
         <f t="shared" si="27"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="891" spans="1:7" x14ac:dyDescent="0.3">
@@ -25857,7 +25857,7 @@
       </c>
       <c r="G894" s="12" t="str">
         <f t="shared" si="27"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="895" spans="1:7" x14ac:dyDescent="0.3">
@@ -25981,7 +25981,7 @@
         <v>Não</v>
       </c>
       <c r="G899" s="12" t="str">
-        <f t="shared" ref="G899:G962" si="29">IF(AND(B899&lt;"31/12/2010",C899="Concurso",D899="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G899:G962" si="29">IF(AND(B899&lt;DATE(2010,12,31),C899="Concurso",D899="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -26307,7 +26307,7 @@
       </c>
       <c r="G912" s="12" t="str">
         <f t="shared" si="29"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="913" spans="1:7" x14ac:dyDescent="0.3">
@@ -27581,7 +27581,7 @@
         <v>Não</v>
       </c>
       <c r="G963" s="12" t="str">
-        <f t="shared" ref="G963:G1026" si="31">IF(AND(B963&lt;"31/12/2010",C963="Concurso",D963="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G963:G1026" si="31">IF(AND(B963&lt;DATE(2010,12,31),C963="Concurso",D963="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -28807,7 +28807,7 @@
       </c>
       <c r="G1012" s="12" t="str">
         <f t="shared" si="31"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="1013" spans="1:7" x14ac:dyDescent="0.3">
@@ -29181,7 +29181,7 @@
         <v>Não</v>
       </c>
       <c r="G1027" s="12" t="str">
-        <f t="shared" ref="G1027:G1090" si="33">IF(AND(B1027&lt;"31/12/2010",C1027="Concurso",D1027="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G1027:G1090" si="33">IF(AND(B1027&lt;DATE(2010,12,31),C1027="Concurso",D1027="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>
@@ -29782,7 +29782,7 @@
       </c>
       <c r="G1051" s="12" t="str">
         <f t="shared" si="33"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="1052" spans="1:7" x14ac:dyDescent="0.3">
@@ -29832,7 +29832,7 @@
       </c>
       <c r="G1053" s="12" t="str">
         <f t="shared" si="33"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="1054" spans="1:7" x14ac:dyDescent="0.3">
@@ -29907,7 +29907,7 @@
       </c>
       <c r="G1056" s="12" t="str">
         <f t="shared" si="33"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="1057" spans="1:7" x14ac:dyDescent="0.3">
@@ -30182,7 +30182,7 @@
       </c>
       <c r="G1067" s="12" t="str">
         <f t="shared" si="33"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="1068" spans="1:7" x14ac:dyDescent="0.3">
@@ -30332,7 +30332,7 @@
       </c>
       <c r="G1073" s="12" t="str">
         <f t="shared" si="33"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="1074" spans="1:7" x14ac:dyDescent="0.3">
@@ -30482,7 +30482,7 @@
       </c>
       <c r="G1079" s="12" t="str">
         <f t="shared" si="33"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="1080" spans="1:7" x14ac:dyDescent="0.3">
@@ -30682,7 +30682,7 @@
       </c>
       <c r="G1087" s="12" t="str">
         <f t="shared" si="33"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="1088" spans="1:7" x14ac:dyDescent="0.3">
@@ -30732,7 +30732,7 @@
       </c>
       <c r="G1089" s="12" t="str">
         <f t="shared" si="33"/>
-        <v>Sim</v>
+        <v>Não</v>
       </c>
     </row>
     <row r="1090" spans="1:7" x14ac:dyDescent="0.3">
@@ -30781,7 +30781,7 @@
         <v>Sim</v>
       </c>
       <c r="G1091" s="12" t="str">
-        <f t="shared" ref="G1091:G1093" si="35">IF(AND(B1091&lt;"31/12/2010",C1091="Concurso",D1091="RJ"),"Sim","Não")</f>
+        <f t="shared" ref="G1091:G1093" si="35">IF(AND(B1091&lt;DATE(2010,12,31),C1091="Concurso",D1091="RJ"),"Sim","Não")</f>
         <v>Não</v>
       </c>
     </row>

</xml_diff>